<commit_message>
Arrumando Excel e pastas
</commit_message>
<xml_diff>
--- a/Especificação do Analytics.xlsx
+++ b/Especificação do Analytics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini\Desktop\OneSolutions\OneSolutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecsa\Documents\Grupo 05\OneSolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B2D563-106D-4AC4-88A4-C8EB16496FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B27E264-AD28-44B8-821C-0308DE114889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9BFF0B1-EFE9-4450-A9D5-1D57A667A204}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9BFF0B1-EFE9-4450-A9D5-1D57A667A204}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,18 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>Temperatura</t>
   </si>
   <si>
     <t>13°C</t>
-  </si>
-  <si>
-    <t>22°C</t>
-  </si>
-  <si>
-    <t>27°C</t>
   </si>
   <si>
     <t>17°C</t>
@@ -102,6 +96,9 @@
   </si>
   <si>
     <t>36°C</t>
+  </si>
+  <si>
+    <t>25°C</t>
   </si>
 </sst>
 </file>
@@ -708,6 +705,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,36 +742,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3237,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC930B6-8A37-43B2-987A-B39BC4A0DF10}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3266,7 +3263,7 @@
   <sheetData>
     <row r="1" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="46"/>
       <c r="D1" s="46"/>
@@ -3279,56 +3276,56 @@
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="30"/>
-      <c r="E2" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="60"/>
-      <c r="R2" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="50"/>
+      <c r="E2" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="57"/>
+      <c r="R2" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="60"/>
     </row>
     <row r="3" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>14</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="43" t="s">
-        <v>10</v>
       </c>
       <c r="V3" s="44"/>
       <c r="W3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3355,10 +3352,10 @@
         <v>0.39</v>
       </c>
       <c r="U4" s="7">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="V4" s="8">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="W4" s="6">
         <v>0.55000000000000004</v>
@@ -3405,16 +3402,16 @@
       <c r="F6" s="25">
         <v>0.52</v>
       </c>
-      <c r="R6" s="48" t="s">
+      <c r="R6" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
-      <c r="V6" s="49"/>
-      <c r="W6" s="49"/>
-      <c r="X6" s="49"/>
-      <c r="Y6" s="50"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="60"/>
     </row>
     <row r="7" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24">
@@ -3431,26 +3428,26 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U7" s="43" t="s">
         <v>8</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U7" s="43" t="s">
-        <v>10</v>
       </c>
       <c r="V7" s="44"/>
       <c r="W7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3471,25 +3468,25 @@
         <v>1</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="W8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="U8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="V8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="W8" s="12" t="s">
-        <v>7</v>
-      </c>
       <c r="X8" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Y8" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3611,14 +3608,14 @@
       <c r="F16" s="25">
         <v>0.38500000000000001</v>
       </c>
-      <c r="J16" s="56" t="s">
+      <c r="J16" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="58"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="24">
@@ -3635,22 +3632,22 @@
         <v>0.39</v>
       </c>
       <c r="J17" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="18" t="s">
+      <c r="N17" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="35" t="s">
         <v>16</v>
-      </c>
-      <c r="M17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17" s="35" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3936,33 +3933,33 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J35" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="53"/>
+      <c r="J35" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="50"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J36" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M36" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" s="18" t="s">
+      <c r="N36" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="O36" s="35" t="s">
         <v>16</v>
-      </c>
-      <c r="M36" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="N36" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="O36" s="35" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>